<commit_message>
Updates for talk at Faithlife.
</commit_message>
<xml_diff>
--- a/WhatWhere.xlsx
+++ b/WhatWhere.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Presentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9494E748-F57F-49C6-BAC3-846E03B6E09D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A23C07-382E-457F-971A-D841993A44BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>Intro to Async</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>CosmosDB</t>
+  </si>
+  <si>
+    <t>Faithlife</t>
+  </si>
+  <si>
+    <t>2021-07</t>
   </si>
 </sst>
 </file>
@@ -459,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +482,7 @@
     <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -510,8 +516,11 @@
       <c r="L1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -522,7 +531,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -538,8 +547,11 @@
       <c r="F3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -553,7 +565,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -573,7 +585,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -584,7 +596,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -595,7 +607,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -603,7 +615,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -611,7 +623,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -625,7 +637,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Async Masterclass at ThatConf 2023
</commit_message>
<xml_diff>
--- a/WhatWhere.xlsx
+++ b/WhatWhere.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Presentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A23C07-382E-457F-971A-D841993A44BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FB3B04-32B6-4C4A-A294-2E5270F6BD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>Intro to Async</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>2021-07</t>
+  </si>
+  <si>
+    <t>Async Masterclass</t>
+  </si>
+  <si>
+    <t>2023-07</t>
   </si>
 </sst>
 </file>
@@ -465,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,6 +651,14 @@
         <v>35</v>
       </c>
     </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>